<commit_message>
Add size tracking functionality, support 2019 sale
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SSENSE_Price_checker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SSENSE_Price_checker\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA9BBA9-4BFC-4E5F-9D8E-574AAA4D692A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12870"/>
+    <workbookView xWindow="3240" yWindow="3497" windowWidth="24686" windowHeight="13149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,39 +25,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>https://www.ssense.com/en-ca/men/product/fendi/blue-bag-bugs-card-holder/2178387</t>
-  </si>
-  <si>
-    <t>https://www.ssense.com/en-ca/men/product/burberry/black-william-boots/2202207</t>
-  </si>
-  <si>
-    <t>https://www.ssense.com/en-ca/men/product/valentino/black-and-green-valentino-garavani-small-rockstud-card-holder/2213067</t>
-  </si>
-  <si>
-    <t>https://www.ssense.com/en-ca/men/product/versace/black-small-medusa-card-holder/2083627</t>
-  </si>
-  <si>
-    <t>https://www.ssense.com/en-ca/men/product/fendi/green-bag-bugs-card-holder/2058007</t>
-  </si>
-  <si>
-    <t>https://www.ssense.com/en-ca/men/product/feit/green-suede-chelsea-boots/1666763</t>
-  </si>
-  <si>
-    <t>https://www.ssense.com/en-ca/men/product/grenson/black-suede-declan-boots/2270267</t>
-  </si>
-  <si>
-    <t>https://www.ssense.com/en-ca/women/product/msgm/white-logo-hoodie/2154147</t>
-  </si>
-  <si>
-    <t>https://www.ssense.com/en-ca/women/product/mcq-alexander-mcqueen/black-bunny-be-here-now-sweatshirt/2049993</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/loewe/white-puzzle-sneakers/3480259</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/common-projects/white-and-orange-original-achilles-retro-low-sneakers/3640649</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/adidas-originals/white-and-grey-ultraboost-19-sneakers/3321519</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/adidas-originals/black-and-white-performance-ultraboost-19-sneakers/3303279</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/acne-studios/white-bla-konst-tennis-sneakers/3701939</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/golden-goose/white-and-black-metal-logo-superstar-sneakers/3618999</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/golden-goose/white-and-silver-superstar-sneakers/3625719</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/golden-goose/yellow-grindstar-sneakers/3508469</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/golden-goose/white-and-orange-superstar-sneakers/3506979</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/givenchy/white-and-red-urban-knots-sneakers/3273369</t>
+  </si>
+  <si>
+    <t>https://www.ssense.com/en-ca/men/product/givenchy/white-and-black-urban-knots-sneakers/3315559</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,7 +113,18 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -415,156 +433,254 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="118.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="118.3046875" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" customWidth="1"/>
+    <col min="3" max="3" width="8.3828125" customWidth="1"/>
+    <col min="4" max="4" width="7.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>217</v>
+        <v>432</v>
       </c>
       <c r="C1">
-        <v>275</v>
+        <v>432</v>
       </c>
       <c r="D1">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>712</v>
+        <v>352</v>
       </c>
       <c r="C2">
-        <v>1095</v>
+        <v>352</v>
       </c>
       <c r="D2">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>270</v>
+        <v>140</v>
       </c>
       <c r="C3">
-        <v>270</v>
+        <v>140</v>
       </c>
       <c r="D3">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="C4">
-        <v>225</v>
+        <v>140</v>
       </c>
       <c r="D4">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>259</v>
+        <v>189</v>
       </c>
       <c r="C5">
-        <v>355</v>
+        <v>189</v>
       </c>
       <c r="D5">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>456</v>
+        <v>382</v>
       </c>
       <c r="C6">
-        <v>1200</v>
+        <v>395</v>
       </c>
       <c r="D6">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+      <c r="E6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>239</v>
+        <v>446</v>
       </c>
       <c r="C7">
-        <v>420</v>
+        <v>468</v>
       </c>
       <c r="D7">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>382</v>
+      </c>
+      <c r="C8">
+        <v>395</v>
+      </c>
+      <c r="D8">
+        <v>382</v>
+      </c>
+      <c r="E8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>229</v>
-      </c>
-      <c r="C8">
-        <v>260</v>
-      </c>
-      <c r="D8">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9">
+        <v>281</v>
+      </c>
+      <c r="C9">
+        <v>281</v>
+      </c>
+      <c r="D9">
+        <v>281</v>
+      </c>
+      <c r="E9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>263</v>
-      </c>
-      <c r="C9">
-        <v>355</v>
-      </c>
-      <c r="D9">
-        <v>263</v>
+      <c r="B10">
+        <v>489</v>
+      </c>
+      <c r="C10">
+        <v>489</v>
+      </c>
+      <c r="D10">
+        <v>489</v>
+      </c>
+      <c r="E10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>371</v>
+      </c>
+      <c r="C11">
+        <v>371</v>
+      </c>
+      <c r="D11">
+        <v>371</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>397</v>
+      </c>
+      <c r="C12">
+        <v>435</v>
+      </c>
+      <c r="D12">
+        <v>397</v>
+      </c>
+      <c r="E12">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>489</v>
+      </c>
+      <c r="C13">
+        <v>489</v>
+      </c>
+      <c r="D13">
+        <v>489</v>
+      </c>
+      <c r="E13">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>$C$1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1"/>
-    <hyperlink ref="A6" r:id="rId2" display="https://urldefense.proofpoint.com/v2/url?u=https-3A__www.ssense.com_en-2Dca_men_product_feit_green-2Dsuede-2Dchelsea-2Dboots_1666763&amp;d=DwMFaQ&amp;c=7T-TmBDHmd8pPB-TR4ileg&amp;r=1TKakADSV0l6fnZJIJ7ZVkd208_PDbNug05RJn_9zNE&amp;m=EArn7QdBK27T0oReGkq8cRLRY5x7zfSIUKKT6UFAtQM&amp;s=8H0rEC0d2b72UAOtA4R9tO4ZrRhVgPIyUkfv0f46Hrk&amp;e="/>
-    <hyperlink ref="A7" r:id="rId3" display="https://urldefense.proofpoint.com/v2/url?u=https-3A__www.ssense.com_en-2Dca_men_product_grenson_black-2Dsuede-2Ddeclan-2Dboots_2270267&amp;d=DwMFaQ&amp;c=7T-TmBDHmd8pPB-TR4ileg&amp;r=1TKakADSV0l6fnZJIJ7ZVkd208_PDbNug05RJn_9zNE&amp;m=EArn7QdBK27T0oReGkq8cRLRY5x7zfSIUKKT6UFAtQM&amp;s=80Lo9mDBjbQCNrbSfp0r46lAthk68E_qwlcgigSRWok&amp;e="/>
-    <hyperlink ref="A8" r:id="rId4" display="https://urldefense.proofpoint.com/v2/url?u=https-3A__www.ssense.com_en-2Dca_women_product_msgm_white-2Dlogo-2Dhoodie_2154147&amp;d=DwMFaQ&amp;c=7T-TmBDHmd8pPB-TR4ileg&amp;r=1TKakADSV0l6fnZJIJ7ZVkd208_PDbNug05RJn_9zNE&amp;m=EArn7QdBK27T0oReGkq8cRLRY5x7zfSIUKKT6UFAtQM&amp;s=aBvSpWzlXc26DoGK23nQsPguq1Zumbz-Nd0ewfZS_Rw&amp;e="/>
-    <hyperlink ref="A9" r:id="rId5" display="https://urldefense.proofpoint.com/v2/url?u=https-3A__www.ssense.com_en-2Dca_women_product_mcq-2Dalexander-2Dmcqueen_black-2Dbunny-2Dbe-2Dhere-2Dnow-2Dsweatshirt_2049993&amp;d=DwMFaQ&amp;c=7T-TmBDHmd8pPB-TR4ileg&amp;r=1TKakADSV0l6fnZJIJ7ZVkd208_PDbNug05RJn_9zNE&amp;m=EArn7QdBK27T0oReGkq8cRLRY5x7zfSIUKKT6UFAtQM&amp;s=jzRR6gfyylAxNq7h1GJFKxz4kL6vjq2-NUC0Mnek7H8&amp;e="/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{FB79A0D9-8CEB-48AA-A90A-FB3DA842EBB4}"/>
+    <hyperlink ref="A1" r:id="rId2" xr:uid="{E2A23388-45C8-4777-936F-972243007B18}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{67E4CF0C-F2CC-4E25-A13E-5AE44B4F69DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>